<commit_message>
david added to some committees...
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@786 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/governance/FMG/FMG Tracking Sheet.xlsx
+++ b/documents/governance/FMG/FMG Tracking Sheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="260" windowWidth="24080" windowHeight="18600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Work Groups" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="222">
   <si>
     <t>Patient Care</t>
   </si>
@@ -1185,7 +1185,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1271,7 +1271,9 @@
       <c r="D3" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F3" s="5" t="s">
         <v>175</v>
       </c>
@@ -1345,7 +1347,9 @@
       <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1373,7 +1377,9 @@
       <c r="D7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F7" s="5" t="s">
         <v>76</v>
       </c>
@@ -1454,7 +1460,9 @@
         <v>141</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>75</v>
       </c>
@@ -1502,7 +1510,9 @@
         <v>139</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F12" s="2" t="s">
         <v>75</v>
       </c>
@@ -1604,7 +1614,9 @@
         <v>136</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>75</v>
       </c>
@@ -1781,7 +1793,9 @@
         <v>4</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F23" s="2" t="s">
         <v>75</v>
       </c>
@@ -1803,7 +1817,9 @@
       <c r="C24" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
Changed resource categories to align with Grahame's current categorizations
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@787 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/governance/FMG/FMG Tracking Sheet.xlsx
+++ b/documents/governance/FMG/FMG Tracking Sheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Work Groups" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="Members">'FMG Members'!$A$2:$A$10</definedName>
     <definedName name="WorkGroups">'Work Groups'!$B$2:$B$26</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="225">
   <si>
     <t>Patient Care</t>
   </si>
@@ -693,6 +693,15 @@
   </si>
   <si>
     <t>Lorraine?</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>Technical</t>
+  </si>
+  <si>
+    <t>Medications</t>
   </si>
 </sst>
 </file>
@@ -1185,24 +1194,24 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="63.1640625" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="7"/>
+    <col min="7" max="7" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="63.140625" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -1231,7 +1240,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>52</v>
       </c>
@@ -1258,7 +1267,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>52</v>
       </c>
@@ -1287,7 +1296,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>52</v>
       </c>
@@ -1312,7 +1321,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1337,7 +1346,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
@@ -1364,7 +1373,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -1393,7 +1402,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1422,7 +1431,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
@@ -1449,7 +1458,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -1474,7 +1483,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
@@ -1524,7 +1533,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
@@ -1553,7 +1562,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1580,7 +1589,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
@@ -1603,7 +1612,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
@@ -1651,7 +1660,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="28">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
@@ -1678,7 +1687,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
@@ -1705,7 +1714,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>10</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>10</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>10</v>
       </c>
@@ -1782,7 +1791,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>10</v>
       </c>
@@ -1807,7 +1816,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>40</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>40</v>
       </c>
@@ -1855,7 +1864,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>40</v>
       </c>
@@ -1878,7 +1887,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
@@ -1889,7 +1898,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>45</v>
       </c>
@@ -1902,7 +1911,7 @@
       <c r="H28" s="21"/>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" ht="28">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
@@ -1919,7 +1928,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="28">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>11</v>
       </c>
@@ -1936,7 +1945,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>11</v>
       </c>
@@ -1953,7 +1962,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="28">
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>11</v>
       </c>
@@ -1970,7 +1979,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>11</v>
       </c>
@@ -1987,7 +1996,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>11</v>
       </c>
@@ -2004,7 +2013,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>11</v>
       </c>
@@ -2021,7 +2030,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>11</v>
       </c>
@@ -2038,7 +2047,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="28">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>11</v>
       </c>
@@ -2055,7 +2064,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>10</v>
       </c>
@@ -2072,7 +2081,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>10</v>
       </c>
@@ -2089,7 +2098,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>10</v>
       </c>
@@ -2106,7 +2115,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>10</v>
       </c>
@@ -2123,7 +2132,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>10</v>
       </c>
@@ -2140,7 +2149,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>40</v>
       </c>
@@ -2157,7 +2166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>40</v>
       </c>
@@ -2174,7 +2183,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>40</v>
       </c>
@@ -2191,7 +2200,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>40</v>
       </c>
@@ -2236,22 +2245,22 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>86</v>
       </c>
@@ -2263,7 +2272,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
     </row>
-    <row r="2" spans="1:8" ht="28">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>159</v>
       </c>
@@ -2289,7 +2298,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>200</v>
       </c>
@@ -2306,7 +2315,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>200</v>
       </c>
@@ -2323,7 +2332,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>200</v>
       </c>
@@ -2340,7 +2349,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>200</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>200</v>
       </c>
@@ -2374,7 +2383,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>200</v>
       </c>
@@ -2391,7 +2400,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>195</v>
       </c>
@@ -2408,7 +2417,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>195</v>
       </c>
@@ -2425,7 +2434,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>195</v>
       </c>
@@ -2439,7 +2448,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>195</v>
       </c>
@@ -2456,7 +2465,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>195</v>
       </c>
@@ -2470,7 +2479,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>195</v>
       </c>
@@ -2487,7 +2496,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -2507,7 +2516,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>180</v>
       </c>
@@ -2524,7 +2533,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>180</v>
       </c>
@@ -2541,7 +2550,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>180</v>
       </c>
@@ -2561,7 +2570,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>180</v>
       </c>
@@ -2581,7 +2590,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>180</v>
       </c>
@@ -2598,7 +2607,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>180</v>
       </c>
@@ -2615,7 +2624,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>180</v>
       </c>
@@ -2632,7 +2641,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>180</v>
       </c>
@@ -2649,7 +2658,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>180</v>
       </c>
@@ -2669,7 +2678,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>180</v>
       </c>
@@ -2689,7 +2698,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>190</v>
       </c>
@@ -2709,7 +2718,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>190</v>
       </c>
@@ -2726,7 +2735,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>190</v>
       </c>
@@ -2746,7 +2755,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>190</v>
       </c>
@@ -2763,7 +2772,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>190</v>
       </c>
@@ -2780,7 +2789,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>190</v>
       </c>
@@ -2797,7 +2806,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>190</v>
       </c>
@@ -2814,7 +2823,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -2834,35 +2843,32 @@
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>190</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="G34" t="s">
         <v>96</v>
       </c>
       <c r="H34" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>190</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="G35" t="s">
         <v>96</v>
@@ -2871,12 +2877,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>190</v>
       </c>
-      <c r="B36" s="17" t="s">
-        <v>112</v>
+      <c r="B36" t="s">
+        <v>113</v>
       </c>
       <c r="C36" t="s">
         <v>111</v>
@@ -2885,78 +2891,78 @@
         <v>96</v>
       </c>
       <c r="H36" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>190</v>
-      </c>
-      <c r="B37" t="s">
-        <v>113</v>
+        <v>188</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>145</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G37" t="s">
         <v>96</v>
       </c>
       <c r="H37" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>211</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
         <v>126</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="G38" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="H38" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>126</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
       </c>
       <c r="G39" t="s">
         <v>96</v>
       </c>
       <c r="H39" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>222</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
         <v>126</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G40" t="s">
         <v>91</v>
@@ -2965,58 +2971,58 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>222</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>95</v>
+        <v>207</v>
       </c>
       <c r="C41" t="s">
         <v>126</v>
       </c>
       <c r="D41" t="s">
-        <v>44</v>
+        <v>212</v>
       </c>
       <c r="G41" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="H41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>222</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="C42" t="s">
         <v>126</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="G42" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H42" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>222</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
         <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="G43" t="s">
         <v>91</v>
@@ -3025,229 +3031,232 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>222</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>93</v>
+        <v>211</v>
       </c>
       <c r="C44" t="s">
         <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>82</v>
+      </c>
+      <c r="E44" t="s">
+        <v>159</v>
       </c>
       <c r="G44" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H44" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>189</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" t="s">
+        <v>103</v>
+      </c>
+      <c r="H45" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
-      <c r="A45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="C45" t="s">
-        <v>126</v>
-      </c>
-      <c r="D45" t="s">
-        <v>212</v>
-      </c>
-      <c r="G45" t="s">
-        <v>41</v>
-      </c>
-      <c r="H45" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>208</v>
+        <v>189</v>
+      </c>
+      <c r="B46" t="s">
+        <v>121</v>
       </c>
       <c r="C46" t="s">
-        <v>126</v>
-      </c>
-      <c r="D46" t="s">
-        <v>212</v>
+        <v>101</v>
       </c>
       <c r="G46" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="H46" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>97</v>
+        <v>224</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
-      </c>
-      <c r="D47" t="s">
-        <v>135</v>
+        <v>2</v>
       </c>
       <c r="G47" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="H47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>224</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>210</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
-      </c>
-      <c r="D48" t="s">
-        <v>82</v>
-      </c>
-      <c r="E48" t="s">
-        <v>213</v>
+        <v>2</v>
       </c>
       <c r="G48" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="H48" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>189</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>104</v>
+        <v>224</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="G49" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>189</v>
+        <v>224</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="H50" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" t="s">
-        <v>115</v>
+        <v>224</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>119</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
+      <c r="E51" t="s">
+        <v>181</v>
+      </c>
       <c r="G51" t="s">
         <v>96</v>
       </c>
       <c r="H51" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>2</v>
+        <v>223</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>126</v>
+      </c>
+      <c r="D52" t="s">
+        <v>44</v>
       </c>
       <c r="G52" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>223</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" t="s">
+        <v>131</v>
+      </c>
+      <c r="G53" t="s">
+        <v>91</v>
+      </c>
+      <c r="H53" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" t="s">
-        <v>2</v>
-      </c>
-      <c r="G53" t="s">
-        <v>96</v>
-      </c>
-      <c r="H53" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" t="s">
-        <v>118</v>
+        <v>223</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>2</v>
+        <v>126</v>
+      </c>
+      <c r="D54" t="s">
+        <v>131</v>
       </c>
       <c r="G54" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H54" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>2</v>
+        <v>223</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>119</v>
+        <v>210</v>
       </c>
       <c r="C55" t="s">
-        <v>2</v>
+        <v>126</v>
+      </c>
+      <c r="D55" t="s">
+        <v>82</v>
       </c>
       <c r="E55" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="G55" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="H55" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3282,54 +3291,54 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>216</v>
       </c>

</xml_diff>

<commit_message>
Updated PHER and added my name to a EHR/CIC
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@840 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/governance/FMG/FMG Tracking Sheet.xlsx
+++ b/documents/governance/FMG/FMG Tracking Sheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15880"/>
   </bookViews>
   <sheets>
     <sheet name="Work Groups" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="Members">'FMG Members'!$A$2:$A$10</definedName>
     <definedName name="WorkGroups">'Work Groups'!$B$2:$B$28</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="231">
   <si>
     <t>Patient Care</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Near term resource development potential</t>
   </si>
   <si>
-    <t>Not likely involved (governance structure)</t>
-  </si>
-  <si>
     <t>May eventually be interested in FHIR for curly brackets potential</t>
   </si>
   <si>
@@ -717,6 +714,12 @@
   </si>
   <si>
     <t>Aim to create a conformance specification for standardization of interface between mobile devices and Electronic Health Records (EHR)/ Personal Health Records (PHR) systems.  Starting 2013/Jan</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Not likely involved (governance structure) - but may use as a source for Requirements</t>
   </si>
 </sst>
 </file>
@@ -1215,29 +1218,29 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="63.140625" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="7"/>
+    <col min="7" max="7" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="63.1640625" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="28">
       <c r="A1" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>49</v>
@@ -1249,27 +1252,27 @@
         <v>50</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>11</v>
@@ -1278,27 +1281,27 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>12</v>
@@ -1310,44 +1313,44 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="9" t="s">
         <v>33</v>
       </c>
@@ -1361,52 +1364,52 @@
         <v>8</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>52</v>
@@ -1421,21 +1424,21 @@
         <v>47</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>10</v>
@@ -1450,21 +1453,21 @@
         <v>47</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>11</v>
@@ -1476,78 +1479,78 @@
         <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>12</v>
@@ -1559,22 +1562,22 @@
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>12</v>
@@ -1586,22 +1589,22 @@
         <v>7</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="42">
       <c r="A14" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>10</v>
@@ -1613,22 +1616,22 @@
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>12</v>
@@ -1643,27 +1646,27 @@
         <v>47</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="42">
       <c r="A16" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>9</v>
@@ -1672,21 +1675,21 @@
         <v>47</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>10</v>
@@ -1701,21 +1704,21 @@
         <v>47</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>11</v>
@@ -1727,19 +1730,19 @@
         <v>8</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
         <v>2</v>
       </c>
@@ -1759,21 +1762,21 @@
         <v>47</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>11</v>
@@ -1782,22 +1785,22 @@
         <v>43</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>162</v>
+        <v>229</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="9" t="s">
         <v>38</v>
       </c>
@@ -1811,25 +1814,25 @@
         <v>9</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>12</v>
@@ -1841,17 +1844,17 @@
         <v>6</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G22" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="9" t="s">
         <v>23</v>
       </c>
@@ -1862,28 +1865,28 @@
         <v>12</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>12</v>
@@ -1895,17 +1898,17 @@
         <v>43</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="9" t="s">
         <v>4</v>
       </c>
@@ -1922,17 +1925,17 @@
         <v>7</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="9" t="s">
         <v>24</v>
       </c>
@@ -1946,20 +1949,20 @@
         <v>9</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="9" t="s">
         <v>39</v>
       </c>
@@ -1970,28 +1973,28 @@
         <v>40</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="28">
       <c r="A28" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>12</v>
@@ -2003,17 +2006,17 @@
         <v>6</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G28" s="15" t="s">
         <v>52</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="12"/>
       <c r="B29" s="11"/>
       <c r="C29" s="10"/>
@@ -2024,7 +2027,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="20" t="s">
@@ -2037,7 +2040,7 @@
       <c r="H30" s="21"/>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="28">
       <c r="A31" s="9" t="s">
         <v>13</v>
       </c>
@@ -2051,10 +2054,10 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="28">
       <c r="A32" s="9" t="s">
         <v>14</v>
       </c>
@@ -2068,10 +2071,10 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="9" t="s">
         <v>15</v>
       </c>
@@ -2085,10 +2088,10 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="28">
       <c r="A34" s="9" t="s">
         <v>16</v>
       </c>
@@ -2102,10 +2105,10 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28">
       <c r="A35" s="9" t="s">
         <v>18</v>
       </c>
@@ -2113,16 +2116,18 @@
       <c r="C35" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="9" t="s">
         <v>19</v>
       </c>
@@ -2136,10 +2141,10 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="9" t="s">
         <v>20</v>
       </c>
@@ -2153,10 +2158,10 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="9" t="s">
         <v>5</v>
       </c>
@@ -2170,10 +2175,10 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="28">
       <c r="A39" s="9" t="s">
         <v>22</v>
       </c>
@@ -2194,7 +2199,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -2208,10 +2213,10 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="9" t="s">
         <v>27</v>
       </c>
@@ -2225,10 +2230,10 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
         <v>28</v>
       </c>
@@ -2242,10 +2247,10 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="9" t="s">
         <v>29</v>
       </c>
@@ -2259,10 +2264,10 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="9" t="s">
         <v>30</v>
       </c>
@@ -2270,16 +2275,20 @@
       <c r="C44" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="9" t="s">
         <v>35</v>
       </c>
@@ -2296,7 +2305,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="9" t="s">
         <v>36</v>
       </c>
@@ -2313,7 +2322,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="9" t="s">
         <v>37</v>
       </c>
@@ -2342,7 +2351,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2362,21 +2371,21 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="20">
       <c r="A1" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -2386,991 +2395,991 @@
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28">
       <c r="A2" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" t="s">
         <v>200</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" t="s">
         <v>204</v>
       </c>
-      <c r="C3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>200</v>
-      </c>
-      <c r="B4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
         <v>201</v>
       </c>
-      <c r="C5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B7" t="s">
-        <v>202</v>
-      </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" t="s">
         <v>195</v>
       </c>
-      <c r="B9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" t="s">
-        <v>135</v>
-      </c>
-      <c r="H9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>195</v>
-      </c>
-      <c r="B10" t="s">
-        <v>199</v>
-      </c>
-      <c r="C10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>195</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>194</v>
       </c>
-      <c r="C11" t="s">
-        <v>126</v>
-      </c>
-      <c r="H11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>195</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>197</v>
       </c>
-      <c r="C12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D12" t="s">
-        <v>130</v>
-      </c>
-      <c r="H12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>195</v>
-      </c>
-      <c r="B13" t="s">
-        <v>196</v>
-      </c>
-      <c r="C13" t="s">
-        <v>126</v>
-      </c>
-      <c r="H13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>195</v>
-      </c>
-      <c r="B14" t="s">
-        <v>198</v>
-      </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" t="s">
         <v>105</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="G15" t="s">
-        <v>106</v>
-      </c>
-      <c r="H15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>149</v>
-      </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G16" t="s">
         <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" t="s">
         <v>102</v>
       </c>
-      <c r="C17" t="s">
-        <v>101</v>
-      </c>
-      <c r="G17" t="s">
-        <v>103</v>
-      </c>
       <c r="H17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" t="s">
         <v>110</v>
       </c>
-      <c r="C18" t="s">
+      <c r="G18" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" t="s">
+        <v>213</v>
+      </c>
+      <c r="H19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" t="s">
         <v>105</v>
       </c>
-      <c r="D18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>180</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="C19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="H21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" t="s">
         <v>105</v>
       </c>
-      <c r="G19" t="s">
-        <v>214</v>
-      </c>
-      <c r="H19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>180</v>
-      </c>
-      <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="H22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" t="s">
         <v>105</v>
       </c>
-      <c r="G20" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>180</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>180</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C22" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" t="s">
-        <v>106</v>
-      </c>
-      <c r="H22" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>180</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" t="s">
-        <v>106</v>
-      </c>
       <c r="H23" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>145</v>
+      </c>
+      <c r="G24" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="G26" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>189</v>
+      </c>
+      <c r="B28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>152</v>
-      </c>
-      <c r="C24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E24" t="s">
-        <v>146</v>
-      </c>
-      <c r="G24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H24" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>180</v>
-      </c>
-      <c r="B25" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" t="s">
-        <v>146</v>
-      </c>
-      <c r="G25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H25" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>190</v>
-      </c>
-      <c r="B26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C26" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="G26" t="s">
-        <v>96</v>
-      </c>
-      <c r="H26" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>190</v>
-      </c>
-      <c r="B27" t="s">
-        <v>114</v>
-      </c>
-      <c r="C27" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H27" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>190</v>
-      </c>
-      <c r="B28" t="s">
-        <v>154</v>
-      </c>
-      <c r="C28" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>153</v>
       </c>
       <c r="G28" t="s">
         <v>41</v>
       </c>
       <c r="H28" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" t="s">
+        <v>95</v>
+      </c>
+      <c r="H31" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" t="s">
+        <v>127</v>
+      </c>
+      <c r="G32" t="s">
+        <v>95</v>
+      </c>
+      <c r="H32" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" t="s">
         <v>182</v>
       </c>
-      <c r="C29" t="s">
+      <c r="G33" t="s">
+        <v>123</v>
+      </c>
+      <c r="H33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>189</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H34" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="G29" t="s">
-        <v>96</v>
-      </c>
-      <c r="H29" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>190</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" t="s">
+        <v>95</v>
+      </c>
+      <c r="H35" t="s">
         <v>185</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" t="s">
         <v>98</v>
       </c>
-      <c r="G30" t="s">
-        <v>96</v>
-      </c>
-      <c r="H30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>190</v>
-      </c>
-      <c r="B31" t="s">
-        <v>184</v>
-      </c>
-      <c r="C31" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" t="s">
-        <v>96</v>
-      </c>
-      <c r="H31" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>190</v>
-      </c>
-      <c r="B32" t="s">
-        <v>120</v>
-      </c>
-      <c r="C32" t="s">
-        <v>128</v>
-      </c>
-      <c r="G32" t="s">
-        <v>96</v>
-      </c>
-      <c r="H32" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>190</v>
-      </c>
-      <c r="B33" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" t="s">
-        <v>183</v>
-      </c>
-      <c r="G33" t="s">
-        <v>124</v>
-      </c>
-      <c r="H33" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>190</v>
-      </c>
-      <c r="B34" s="17" t="s">
+      <c r="G37" t="s">
+        <v>95</v>
+      </c>
+      <c r="H37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>220</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
         <v>125</v>
       </c>
-      <c r="C34" t="s">
-        <v>101</v>
-      </c>
-      <c r="G34" t="s">
-        <v>96</v>
-      </c>
-      <c r="H34" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" t="s">
-        <v>111</v>
-      </c>
-      <c r="G35" t="s">
-        <v>96</v>
-      </c>
-      <c r="H35" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>190</v>
-      </c>
-      <c r="B36" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" t="s">
-        <v>111</v>
-      </c>
-      <c r="G36" t="s">
-        <v>96</v>
-      </c>
-      <c r="H36" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>188</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" t="s">
-        <v>99</v>
-      </c>
-      <c r="G37" t="s">
-        <v>96</v>
-      </c>
-      <c r="H37" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>221</v>
-      </c>
-      <c r="B38" s="17" t="s">
+      <c r="D38" t="s">
+        <v>142</v>
+      </c>
+      <c r="G38" t="s">
         <v>90</v>
       </c>
-      <c r="C38" t="s">
-        <v>126</v>
-      </c>
-      <c r="D38" t="s">
-        <v>143</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>91</v>
       </c>
-      <c r="H38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D39" t="s">
         <v>44</v>
       </c>
       <c r="G39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H39" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G40" t="s">
+        <v>90</v>
+      </c>
+      <c r="H40" t="s">
         <v>91</v>
       </c>
-      <c r="H40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G41" t="s">
         <v>41</v>
       </c>
       <c r="H41" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" t="s">
+        <v>211</v>
+      </c>
+      <c r="G42" t="s">
+        <v>81</v>
+      </c>
+      <c r="H42" t="s">
         <v>208</v>
       </c>
-      <c r="C42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" t="s">
-        <v>212</v>
-      </c>
-      <c r="G42" t="s">
-        <v>82</v>
-      </c>
-      <c r="H42" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G43" t="s">
+        <v>90</v>
+      </c>
+      <c r="H43" t="s">
         <v>91</v>
       </c>
-      <c r="H43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H44" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" t="s">
+        <v>100</v>
+      </c>
+      <c r="G46" t="s">
         <v>121</v>
       </c>
-      <c r="C46" t="s">
-        <v>101</v>
-      </c>
-      <c r="G46" t="s">
-        <v>122</v>
-      </c>
       <c r="H46" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="G47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H47" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="G48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H48" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="G49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H49" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H50" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H51" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D52" t="s">
         <v>44</v>
       </c>
       <c r="G52" t="s">
+        <v>90</v>
+      </c>
+      <c r="H52" t="s">
         <v>91</v>
       </c>
-      <c r="H52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G53" t="s">
+        <v>90</v>
+      </c>
+      <c r="H53" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>221</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" t="s">
+        <v>130</v>
+      </c>
+      <c r="G54" t="s">
+        <v>90</v>
+      </c>
+      <c r="H54" t="s">
         <v>91</v>
       </c>
-      <c r="H53" t="s">
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>221</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>222</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" t="s">
-        <v>126</v>
-      </c>
-      <c r="D54" t="s">
-        <v>131</v>
-      </c>
-      <c r="G54" t="s">
-        <v>91</v>
-      </c>
-      <c r="H54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>222</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="C55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3405,56 +3414,56 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates from FMG session
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@854 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/governance/FMG/FMG Tracking Sheet.xlsx
+++ b/documents/governance/FMG/FMG Tracking Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15885" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Work Groups" sheetId="3" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="FMG Members" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Resources!$A$2:$H$55</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Work Groups'!$A$1:$I$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Resources!$A$2:$H$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Work Groups'!$A$1:$I$32</definedName>
     <definedName name="Members">'FMG Members'!$A$2:$A$10</definedName>
-    <definedName name="WorkGroups">'Work Groups'!$B$2:$B$28</definedName>
+    <definedName name="WorkGroups">'Work Groups'!$B$2:$B$32</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="252">
   <si>
     <t>Patient Care</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Health Care Devices</t>
   </si>
   <si>
-    <t>Regulated Clinical Research Information Management (RCRIM)</t>
-  </si>
-  <si>
     <t>Security</t>
   </si>
   <si>
@@ -110,18 +107,12 @@
     <t>Arden Syntax</t>
   </si>
   <si>
-    <t>Clinical Context Object Workgroup (CCOW)</t>
-  </si>
-  <si>
     <t>Clinical Decision Support</t>
   </si>
   <si>
     <t>Clinical Statement</t>
   </si>
   <si>
-    <t>Electronic Health Record (EHR)</t>
-  </si>
-  <si>
     <t>Imaging Integration</t>
   </si>
   <si>
@@ -305,12 +296,6 @@
     <t>Profile</t>
   </si>
   <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>Document</t>
-  </si>
-  <si>
     <t>CCDA</t>
   </si>
   <si>
@@ -380,9 +365,6 @@
     <t>MedicationStatement</t>
   </si>
   <si>
-    <t>Prescription</t>
-  </si>
-  <si>
     <t>Immunization</t>
   </si>
   <si>
@@ -488,9 +470,6 @@
     <t>AdverseReaction</t>
   </si>
   <si>
-    <t>Merge w/ Allergy?</t>
-  </si>
-  <si>
     <t>IssueReport</t>
   </si>
   <si>
@@ -569,9 +548,6 @@
     <t>Need better name</t>
   </si>
   <si>
-    <t>ImagingObservation</t>
-  </si>
-  <si>
     <t>FamilyHistory</t>
   </si>
   <si>
@@ -647,12 +623,6 @@
     <t>1st ballot</t>
   </si>
   <si>
-    <t>XdsEntry</t>
-  </si>
-  <si>
-    <t>XdsFolder</t>
-  </si>
-  <si>
     <t>Security, IHE</t>
   </si>
   <si>
@@ -717,6 +687,102 @@
   </si>
   <si>
     <t>Was Agent</t>
+  </si>
+  <si>
+    <t>CIMI</t>
+  </si>
+  <si>
+    <t>Clinical Information Modeling Initiative</t>
+  </si>
+  <si>
+    <t>Non-medication - Lloyd to review</t>
+  </si>
+  <si>
+    <t>Figure out better name</t>
+  </si>
+  <si>
+    <t>Was XdsFolder</t>
+  </si>
+  <si>
+    <t>Deferred</t>
+  </si>
+  <si>
+    <t>Was XdsEntry</t>
+  </si>
+  <si>
+    <t>Was Document</t>
+  </si>
+  <si>
+    <t>DocumentRoot</t>
+  </si>
+  <si>
+    <t>MessageRoot</t>
+  </si>
+  <si>
+    <t>Was Message</t>
+  </si>
+  <si>
+    <t>Was Prescription</t>
+  </si>
+  <si>
+    <t>OrderRequest</t>
+  </si>
+  <si>
+    <t>OrderResponse</t>
+  </si>
+  <si>
+    <t>Ewout</t>
+  </si>
+  <si>
+    <t>Ewout Merge w/ Allergy?</t>
+  </si>
+  <si>
+    <t>Imaging[TBD]</t>
+  </si>
+  <si>
+    <t>DeviceManifest</t>
+  </si>
+  <si>
+    <t>DeviceEvent</t>
+  </si>
+  <si>
+    <t>DeviceObservations</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>EHR</t>
+  </si>
+  <si>
+    <t>Electronic Health Record</t>
+  </si>
+  <si>
+    <t>CIC</t>
+  </si>
+  <si>
+    <t>RCRIM</t>
+  </si>
+  <si>
+    <t>Regulated Clinical Research Information Management</t>
+  </si>
+  <si>
+    <t>CCOW</t>
+  </si>
+  <si>
+    <t>Clinical Context Object Workgroup</t>
+  </si>
+  <si>
+    <t>CBCC</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>Arden</t>
   </si>
 </sst>
 </file>
@@ -755,7 +821,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -777,6 +843,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -845,7 +917,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -905,12 +977,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1212,13 +1285,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,896 +1310,922 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B3" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="2"/>
+      <c r="E3" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="I3" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>171</v>
+        <v>18</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>171</v>
+        <v>243</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>6</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>211</v>
+      <c r="E5" s="23" t="s">
+        <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>34</v>
+        <v>164</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>223</v>
+        <v>164</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>211</v>
+        <v>49</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="6" t="s">
-        <v>220</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
+      <c r="E7" s="23" t="s">
+        <v>201</v>
+      </c>
       <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>162</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>167</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="6" t="s">
-        <v>71</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>21</v>
+        <v>242</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>125</v>
+        <v>241</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="24" t="s">
-        <v>6</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="6" t="s">
-        <v>169</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="E10" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>163</v>
+        <v>44</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>211</v>
+      <c r="D11" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="I11" s="6" t="s">
-        <v>168</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>138</v>
+        <v>21</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>6</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="6" t="s">
-        <v>76</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="24" t="s">
-        <v>7</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>156</v>
+      </c>
       <c r="I13" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>221</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>222</v>
+        <v>93</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>8</v>
+      <c r="D14" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="6" t="s">
-        <v>225</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>9</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>224</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="2"/>
       <c r="I16" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>103</v>
+        <v>212</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>9</v>
+      <c r="E17" s="23" t="s">
+        <v>8</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>170</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="6" t="s">
-        <v>70</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>159</v>
+        <v>44</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>43</v>
+        <v>10</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>6</v>
+        <v>44</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>214</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>140</v>
+        <v>1</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>216</v>
+        <v>10</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>226</v>
+        <v>153</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>166</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>216</v>
+      <c r="E21" s="23" t="s">
+        <v>8</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="I21" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>135</v>
+        <v>2</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>131</v>
+        <v>2</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>6</v>
       </c>
+      <c r="E22" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="F22" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H22" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="I22" s="6" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>206</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H23" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="I23" s="6" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>134</v>
+        <v>35</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>206</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>4</v>
+        <v>245</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>44</v>
+        <v>244</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="E25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="6" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>211</v>
+      <c r="D26" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>6</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>6</v>
+      <c r="D28" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="14"/>
+      <c r="A29" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="22"/>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="C31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>49</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="C32" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>49</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="A33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8" t="s">
@@ -2138,12 +2237,12 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8" t="s">
@@ -2155,12 +2254,12 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
@@ -2175,34 +2274,34 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>248</v>
+      </c>
       <c r="C39" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>250</v>
+      </c>
       <c r="C40" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2210,16 +2309,18 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>249</v>
+      </c>
       <c r="C41" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2232,9 +2333,11 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>251</v>
+      </c>
       <c r="C42" s="8" t="s">
         <v>10</v>
       </c>
@@ -2244,14 +2347,16 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="8"/>
+        <v>247</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>246</v>
+      </c>
       <c r="C43" s="8" t="s">
         <v>10</v>
       </c>
@@ -2261,37 +2366,33 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2299,16 +2400,16 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2316,16 +2417,16 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2333,17 +2434,34 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I28">
+  <autoFilter ref="A1:I32">
     <sortState ref="A2:I28">
       <sortCondition ref="A1:A28"/>
     </sortState>
   </autoFilter>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E29 D31:E47">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E33 D35:E41 D42:E48">
       <formula1>Members</formula1>
     </dataValidation>
   </dataValidations>
@@ -2359,13 +2477,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2376,1038 +2495,1155 @@
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="A1" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E2" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>183</v>
-      </c>
       <c r="G2" s="19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H4" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B11" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B13" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G17" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H17" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H18" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G19" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="H19" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H20" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G21" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H21" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G22" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H22" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="G23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H23" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E24" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H24" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" t="s">
-        <v>144</v>
+        <v>94</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>222</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H25" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>153</v>
+        <v>235</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H26" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>104</v>
+      </c>
+      <c r="E27" t="s">
+        <v>234</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D28" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H28" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B29" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>104</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H29" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>186</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>181</v>
+        <v>239</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="G30" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H30" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
+        <v>237</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="G31" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H31" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>238</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G32" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H32" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="H33" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>186</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>123</v>
+        <v>178</v>
+      </c>
+      <c r="B34" t="s">
+        <v>236</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>223</v>
       </c>
       <c r="G34" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H34" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>186</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>110</v>
+        <v>178</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
-      </c>
-      <c r="D35" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="G35" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H35" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>104</v>
+      </c>
+      <c r="E36" t="s">
+        <v>172</v>
       </c>
       <c r="G36" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="H36" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G37" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H37" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="G38" t="s">
         <v>89</v>
       </c>
       <c r="H38" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>217</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>155</v>
+        <v>178</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D39" t="s">
-        <v>109</v>
+        <v>104</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
-      </c>
-      <c r="D40" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="G40" t="s">
         <v>89</v>
       </c>
       <c r="H40" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>203</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>208</v>
+        <v>135</v>
       </c>
       <c r="G41" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="H41" t="s">
-        <v>205</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>204</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D42" t="s">
-        <v>208</v>
+        <v>104</v>
       </c>
       <c r="G42" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="H42" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>95</v>
+        <v>232</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>94</v>
       </c>
       <c r="G43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H43" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="C44" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
-        <v>80</v>
-      </c>
-      <c r="E44" t="s">
-        <v>156</v>
+        <v>94</v>
       </c>
       <c r="G44" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H44" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>118</v>
+      </c>
+      <c r="D45" t="s">
+        <v>136</v>
       </c>
       <c r="G45" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="H45" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>185</v>
-      </c>
-      <c r="B46" t="s">
-        <v>119</v>
+        <v>207</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>195</v>
       </c>
       <c r="C46" t="s">
-        <v>99</v>
+        <v>118</v>
+      </c>
+      <c r="D46" t="s">
+        <v>198</v>
       </c>
       <c r="G46" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="H46" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>219</v>
-      </c>
-      <c r="B47" t="s">
-        <v>113</v>
+        <v>207</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>118</v>
+      </c>
+      <c r="D47" t="s">
+        <v>198</v>
       </c>
       <c r="G47" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="H47" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>118</v>
+      </c>
+      <c r="D48" t="s">
+        <v>127</v>
       </c>
       <c r="G48" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H48" t="s">
-        <v>205</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>219</v>
-      </c>
-      <c r="B49" t="s">
-        <v>115</v>
+        <v>207</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>149</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>118</v>
+      </c>
+      <c r="D49" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" t="s">
+        <v>224</v>
       </c>
       <c r="G49" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="H49" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>219</v>
-      </c>
-      <c r="B50" t="s">
-        <v>116</v>
+        <v>177</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="G50" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H50" t="s">
-        <v>214</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>219</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>117</v>
+        <v>177</v>
+      </c>
+      <c r="B51" t="s">
+        <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
-      </c>
-      <c r="E51" t="s">
-        <v>177</v>
+        <v>94</v>
       </c>
       <c r="G51" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="H51" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>218</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>93</v>
+        <v>209</v>
+      </c>
+      <c r="B52" t="s">
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>124</v>
-      </c>
-      <c r="D52" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="G52" t="s">
         <v>89</v>
       </c>
       <c r="H52" t="s">
-        <v>90</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>154</v>
+        <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>124</v>
-      </c>
-      <c r="D53" t="s">
-        <v>129</v>
+        <v>2</v>
       </c>
       <c r="G53" t="s">
         <v>89</v>
       </c>
       <c r="H53" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>218</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>92</v>
+        <v>209</v>
+      </c>
+      <c r="B54" t="s">
+        <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>124</v>
-      </c>
-      <c r="D54" t="s">
-        <v>129</v>
+        <v>2</v>
       </c>
       <c r="G54" t="s">
         <v>89</v>
       </c>
       <c r="H54" t="s">
-        <v>90</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>218</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>206</v>
+        <v>209</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
-      </c>
-      <c r="D55" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="G55" t="s">
+        <v>89</v>
+      </c>
+      <c r="H55" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>209</v>
       </c>
-      <c r="G55" t="s">
-        <v>80</v>
-      </c>
-      <c r="H55" t="s">
-        <v>205</v>
+      <c r="B56" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>231</v>
+      </c>
+      <c r="G56" t="s">
+        <v>89</v>
+      </c>
+      <c r="H56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>208</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C57" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" t="s">
+        <v>227</v>
+      </c>
+      <c r="G57" t="s">
+        <v>86</v>
+      </c>
+      <c r="H57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>208</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" t="s">
+        <v>118</v>
+      </c>
+      <c r="D58" t="s">
+        <v>123</v>
+      </c>
+      <c r="G58" t="s">
+        <v>86</v>
+      </c>
+      <c r="H58" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>208</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C59" t="s">
+        <v>118</v>
+      </c>
+      <c r="D59" t="s">
+        <v>123</v>
+      </c>
+      <c r="E59" t="s">
+        <v>230</v>
+      </c>
+      <c r="G59" t="s">
+        <v>86</v>
+      </c>
+      <c r="H59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>208</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C60" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" t="s">
+        <v>77</v>
+      </c>
+      <c r="E60" t="s">
+        <v>226</v>
+      </c>
+      <c r="G60" t="s">
+        <v>77</v>
+      </c>
+      <c r="H60" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H55">
+  <autoFilter ref="A2:H60">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="1st ballot"/>
+        <filter val="Draft"/>
+        <filter val="Proposed"/>
+        <filter val="Semi-stable"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A3:H55">
       <sortCondition ref="A3:A55"/>
       <sortCondition ref="B3:B55"/>
@@ -3417,7 +3653,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:C55">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:C60">
       <formula1>WorkGroups</formula1>
     </dataValidation>
   </dataValidations>
@@ -3442,7 +3678,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -3462,17 +3698,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -3482,12 +3718,12 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched primary and backup for II, as agreed with John M
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@862 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/governance/FMG/FMG Tracking Sheet.xlsx
+++ b/documents/governance/FMG/FMG Tracking Sheet.xlsx
@@ -980,10 +980,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1291,7 +1291,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,10 +1672,10 @@
         <v>10</v>
       </c>
       <c r="D14" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="E14" s="23" t="s">
         <v>206</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>201</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>71</v>
@@ -2460,7 +2460,7 @@
       <sortCondition ref="A1:A28"/>
     </sortState>
   </autoFilter>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E33 D35:E41 D42:E48">
       <formula1>Members</formula1>
     </dataValidation>
@@ -2500,16 +2500,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -2933,7 +2933,7 @@
       <c r="C25" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="24" t="s">
         <v>222</v>
       </c>
       <c r="G25" t="s">
@@ -3113,7 +3113,7 @@
       <c r="C34" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="24" t="s">
         <v>223</v>
       </c>
       <c r="G34" t="s">

</xml_diff>

<commit_message>
Updates from FMG call
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@952 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/governance/FMG/FMG Tracking Sheet.xlsx
+++ b/documents/governance/FMG/FMG Tracking Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="253">
   <si>
     <t>Patient Care</t>
   </si>
@@ -783,6 +783,9 @@
   </si>
   <si>
     <t>Arden</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1294,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,8 +1350,12 @@
       <c r="C2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="F2" s="23" t="s">
         <v>71</v>
       </c>
@@ -1400,7 +1407,9 @@
       <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>71</v>
       </c>
@@ -1817,8 +1826,8 @@
       <c r="F19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>153</v>
+      <c r="G19" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>214</v>
@@ -1986,7 +1995,9 @@
       <c r="E25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>252</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="6" t="s">

</xml_diff>

<commit_message>
Added tracking information per resource
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1010 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/governance/FMG/FMG Tracking Sheet.xlsx
+++ b/documents/governance/FMG/FMG Tracking Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="9210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Work Groups" sheetId="3" r:id="rId1"/>
@@ -12,8 +12,8 @@
     <sheet name="FMG Members" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Resources!$A$2:$H$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Work Groups'!$A$1:$I$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Resources!$A$2:$H$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Work Groups'!$A$1:$I$32</definedName>
     <definedName name="Members">'FMG Members'!$A$2:$A$10</definedName>
     <definedName name="WorkGroups">'Work Groups'!$B$2:$B$32</definedName>
   </definedNames>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="268">
   <si>
     <t>Patient Care</t>
   </si>
@@ -786,13 +786,58 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Content Sources</t>
+  </si>
+  <si>
+    <t>Example uses</t>
+  </si>
+  <si>
+    <t>Search Criteria</t>
+  </si>
+  <si>
+    <t>Core elements</t>
+  </si>
+  <si>
+    <t>Examples</t>
+  </si>
+  <si>
+    <t>Element definitions</t>
+  </si>
+  <si>
+    <t>Bindings</t>
+  </si>
+  <si>
+    <t>Requirements &amp; Usage</t>
+  </si>
+  <si>
+    <t>Value Sets / Code Lists</t>
+  </si>
+  <si>
+    <t>Invariants</t>
+  </si>
+  <si>
+    <t>HTML files</t>
+  </si>
+  <si>
+    <t>Mappings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,8 +868,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -852,6 +904,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,7 +978,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -987,11 +1045,154 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1288,13 +1489,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,7 +1542,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>221</v>
       </c>
@@ -1394,7 +1596,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
@@ -1421,7 +1623,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>133</v>
       </c>
@@ -1448,7 +1650,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>164</v>
       </c>
@@ -1475,7 +1677,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>30</v>
       </c>
@@ -1502,7 +1704,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>31</v>
       </c>
@@ -1529,7 +1731,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>242</v>
       </c>
@@ -1614,7 +1816,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -1641,7 +1843,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>77</v>
       </c>
@@ -1670,7 +1872,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
@@ -1697,7 +1899,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>132</v>
       </c>
@@ -1724,7 +1926,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>131</v>
       </c>
@@ -1751,7 +1953,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>211</v>
       </c>
@@ -1865,7 +2067,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>0</v>
       </c>
@@ -1952,7 +2154,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>35</v>
       </c>
@@ -1979,7 +2181,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>245</v>
       </c>
@@ -2004,7 +2206,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>129</v>
       </c>
@@ -2031,7 +2233,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>22</v>
       </c>
@@ -2058,7 +2260,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>128</v>
       </c>
@@ -2085,7 +2287,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>4</v>
       </c>
@@ -2112,7 +2314,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>23</v>
       </c>
@@ -2139,7 +2341,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>36</v>
       </c>
@@ -2166,7 +2368,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>24</v>
       </c>
@@ -2467,6 +2669,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I32">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Developing"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:I28">
       <sortCondition ref="A1:A28"/>
     </sortState>
@@ -2489,13 +2696,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2508,9 +2715,17 @@
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" customWidth="1"/>
+    <col min="24" max="16384" width="8.85546875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>81</v>
       </c>
@@ -2521,8 +2736,16 @@
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I1" s="30">
+        <f ca="1">TODAY()</f>
+        <v>41330</v>
+      </c>
+      <c r="J1" s="30">
+        <f ca="1">DATE(YEAR($I$1),MONTH($I$1)-1,DAY($I$1))</f>
+        <v>41299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>149</v>
       </c>
@@ -2547,47 +2770,176 @@
       <c r="H2" s="19" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I2" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29">
+        <v>41334</v>
+      </c>
+      <c r="J3" s="29">
+        <v>41334</v>
+      </c>
+      <c r="K3" s="29">
+        <v>41334</v>
+      </c>
+      <c r="L3" s="29">
+        <v>41334</v>
+      </c>
+      <c r="M3" s="29">
+        <v>41365</v>
+      </c>
+      <c r="N3" s="29">
+        <v>41365</v>
+      </c>
+      <c r="O3" s="29">
+        <v>41365</v>
+      </c>
+      <c r="P3" s="29">
+        <v>41395</v>
+      </c>
+      <c r="Q3" s="29">
+        <v>41395</v>
+      </c>
+      <c r="R3" s="29">
+        <v>41395</v>
+      </c>
+      <c r="S3" s="29">
+        <v>41395</v>
+      </c>
+      <c r="T3" s="29">
+        <v>41395</v>
+      </c>
+      <c r="U3" s="29">
+        <v>41395</v>
+      </c>
+      <c r="V3" s="29">
+        <v>41395</v>
+      </c>
+      <c r="W3" s="29">
+        <v>41395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="29">
+        <v>41365</v>
+      </c>
+      <c r="J4" s="29">
+        <v>41365</v>
+      </c>
+      <c r="K4" s="29">
+        <v>41365</v>
+      </c>
+      <c r="L4" s="29">
+        <v>41365</v>
+      </c>
+      <c r="M4" s="29">
+        <v>41395</v>
+      </c>
+      <c r="N4" s="29">
+        <v>41395</v>
+      </c>
+      <c r="O4" s="29">
+        <v>41395</v>
+      </c>
+      <c r="P4" s="29">
+        <v>41456</v>
+      </c>
+      <c r="Q4" s="29">
+        <v>41456</v>
+      </c>
+      <c r="R4" s="29">
+        <v>41456</v>
+      </c>
+      <c r="S4" s="29">
+        <v>41456</v>
+      </c>
+      <c r="T4" s="29">
+        <v>41456</v>
+      </c>
+      <c r="U4" s="29">
+        <v>41456</v>
+      </c>
+      <c r="V4" s="29">
+        <v>41456</v>
+      </c>
+      <c r="W4" s="29">
+        <v>41456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
         <v>118</v>
@@ -2599,29 +2951,29 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C6" t="s">
         <v>118</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
@@ -2633,77 +2985,80 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>188</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
         <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="H8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
         <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>118</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>183</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C11" t="s">
         <v>118</v>
       </c>
+      <c r="D11" t="s">
+        <v>127</v>
+      </c>
       <c r="H11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>183</v>
       </c>
       <c r="B12" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C12" t="s">
         <v>118</v>
@@ -2715,12 +3070,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>183</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
         <v>118</v>
@@ -2729,61 +3084,52 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>183</v>
       </c>
       <c r="B14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C14" t="s">
         <v>118</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>140</v>
+        <v>183</v>
+      </c>
+      <c r="B15" t="s">
+        <v>184</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" t="s">
-        <v>219</v>
-      </c>
-      <c r="G15" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="H15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>169</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>141</v>
+        <v>183</v>
+      </c>
+      <c r="B16" t="s">
+        <v>186</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" t="s">
-        <v>218</v>
-      </c>
-      <c r="G16" t="s">
-        <v>38</v>
+        <v>118</v>
+      </c>
+      <c r="D16" t="s">
+        <v>127</v>
       </c>
       <c r="H16" t="s">
-        <v>218</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2791,36 +3137,39 @@
         <v>169</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
+        <v>219</v>
       </c>
       <c r="G17" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H17" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>169</v>
       </c>
-      <c r="B18" t="s">
-        <v>103</v>
+      <c r="B18" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="C18" t="s">
         <v>98</v>
       </c>
-      <c r="D18" t="s">
-        <v>104</v>
+      <c r="E18" t="s">
+        <v>218</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="H18" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2828,19 +3177,16 @@
         <v>169</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>194</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G19" t="s">
-        <v>200</v>
+        <v>96</v>
       </c>
       <c r="H19" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2848,10 +3194,13 @@
         <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
         <v>98</v>
+      </c>
+      <c r="D20" t="s">
+        <v>104</v>
       </c>
       <c r="G20" t="s">
         <v>89</v>
@@ -2865,13 +3214,16 @@
         <v>169</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>100</v>
+        <v>194</v>
       </c>
       <c r="C21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" t="s">
         <v>98</v>
       </c>
       <c r="G21" t="s">
-        <v>99</v>
+        <v>200</v>
       </c>
       <c r="H21" t="s">
         <v>197</v>
@@ -2881,94 +3233,85 @@
       <c r="A22" t="s">
         <v>169</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>101</v>
+      <c r="B22" t="s">
+        <v>102</v>
       </c>
       <c r="C22" t="s">
         <v>98</v>
       </c>
       <c r="G22" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="H22" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>169</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
         <v>98</v>
       </c>
-      <c r="E23" t="s">
-        <v>218</v>
-      </c>
       <c r="G23" t="s">
         <v>99</v>
       </c>
       <c r="H23" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>169</v>
       </c>
-      <c r="B24" t="s">
-        <v>143</v>
+      <c r="B24" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="G24" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="H24" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>169</v>
       </c>
-      <c r="B25" t="s">
-        <v>139</v>
+      <c r="B25" s="17" t="s">
+        <v>142</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>222</v>
+        <v>98</v>
+      </c>
+      <c r="E25" t="s">
+        <v>218</v>
       </c>
       <c r="G25" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="H25" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>235</v>
+        <v>94</v>
+      </c>
+      <c r="E26" t="s">
+        <v>138</v>
       </c>
       <c r="G26" t="s">
         <v>89</v>
@@ -2979,19 +3322,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" t="s">
-        <v>234</v>
+        <v>94</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>222</v>
       </c>
       <c r="G27" t="s">
         <v>89</v>
@@ -3000,12 +3340,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>178</v>
       </c>
       <c r="B28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C28" t="s">
         <v>118</v>
@@ -3014,13 +3354,13 @@
         <v>104</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>144</v>
+        <v>235</v>
       </c>
       <c r="G28" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="H28" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3028,7 +3368,7 @@
         <v>178</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="C29" t="s">
         <v>118</v>
@@ -3037,7 +3377,7 @@
         <v>104</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>234</v>
       </c>
       <c r="G29" t="s">
         <v>89</v>
@@ -3046,35 +3386,47 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>239</v>
+        <v>145</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="D30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>144</v>
       </c>
       <c r="G30" t="s">
-        <v>240</v>
+        <v>38</v>
       </c>
       <c r="H30" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="B31" t="s">
-        <v>237</v>
+        <v>171</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="D31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>240</v>
+        <v>89</v>
       </c>
       <c r="H31" t="s">
         <v>204</v>
@@ -3085,7 +3437,7 @@
         <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C32" t="s">
         <v>119</v>
@@ -3099,16 +3451,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>173</v>
+        <v>237</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="G33" t="s">
-        <v>89</v>
+        <v>240</v>
       </c>
       <c r="H33" t="s">
         <v>204</v>
@@ -3116,19 +3468,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>223</v>
+        <v>119</v>
       </c>
       <c r="G34" t="s">
-        <v>89</v>
+        <v>240</v>
       </c>
       <c r="H34" t="s">
         <v>204</v>
@@ -3139,10 +3488,10 @@
         <v>178</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>173</v>
       </c>
       <c r="C35" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="G35" t="s">
         <v>89</v>
@@ -3151,52 +3500,49 @@
         <v>204</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>178</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>236</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36" t="s">
-        <v>104</v>
-      </c>
-      <c r="E36" t="s">
-        <v>172</v>
+        <v>93</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>223</v>
       </c>
       <c r="G36" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="H36" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>178</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>117</v>
+      <c r="B37" t="s">
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="G37" t="s">
         <v>89</v>
       </c>
       <c r="H37" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>178</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>105</v>
+      <c r="B38" t="s">
+        <v>115</v>
       </c>
       <c r="C38" t="s">
         <v>118</v>
@@ -3204,45 +3550,45 @@
       <c r="D38" t="s">
         <v>104</v>
       </c>
+      <c r="E38" t="s">
+        <v>172</v>
+      </c>
       <c r="G38" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="H38" t="s">
-        <v>174</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>178</v>
       </c>
-      <c r="B39" t="s">
-        <v>106</v>
+      <c r="B39" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="G39" t="s">
         <v>89</v>
       </c>
       <c r="H39" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>118</v>
+      </c>
+      <c r="D40" t="s">
+        <v>104</v>
       </c>
       <c r="G40" t="s">
         <v>89</v>
@@ -3253,42 +3599,42 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>207</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>85</v>
+        <v>178</v>
+      </c>
+      <c r="B41" t="s">
+        <v>106</v>
       </c>
       <c r="C41" t="s">
         <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>104</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
       </c>
       <c r="G41" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H41" t="s">
-        <v>87</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>207</v>
+        <v>176</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G42" t="s">
         <v>89</v>
       </c>
       <c r="H42" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3296,19 +3642,19 @@
         <v>207</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>232</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
         <v>118</v>
       </c>
       <c r="D43" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="G43" t="s">
         <v>86</v>
       </c>
       <c r="H43" t="s">
-        <v>174</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3316,19 +3662,19 @@
         <v>207</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="C44" t="s">
         <v>118</v>
       </c>
       <c r="D44" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G44" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H44" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3336,19 +3682,19 @@
         <v>207</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>88</v>
+        <v>232</v>
       </c>
       <c r="C45" t="s">
         <v>118</v>
       </c>
       <c r="D45" t="s">
-        <v>136</v>
+        <v>94</v>
       </c>
       <c r="G45" t="s">
         <v>86</v>
       </c>
       <c r="H45" t="s">
-        <v>87</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3356,19 +3702,19 @@
         <v>207</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>195</v>
+        <v>233</v>
       </c>
       <c r="C46" t="s">
         <v>118</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>94</v>
       </c>
       <c r="G46" t="s">
         <v>86</v>
       </c>
       <c r="H46" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3376,19 +3722,19 @@
         <v>207</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>196</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
         <v>118</v>
       </c>
       <c r="D47" t="s">
-        <v>198</v>
+        <v>136</v>
       </c>
       <c r="G47" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="H47" t="s">
-        <v>197</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3396,19 +3742,19 @@
         <v>207</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
       <c r="C48" t="s">
         <v>118</v>
       </c>
       <c r="D48" t="s">
-        <v>127</v>
+        <v>198</v>
       </c>
       <c r="G48" t="s">
         <v>86</v>
       </c>
       <c r="H48" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3416,16 +3762,13 @@
         <v>207</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C49" t="s">
         <v>118</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
-      </c>
-      <c r="E49" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="G49" t="s">
         <v>77</v>
@@ -3436,16 +3779,19 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>118</v>
+      </c>
+      <c r="D50" t="s">
+        <v>127</v>
       </c>
       <c r="G50" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H50" t="s">
         <v>87</v>
@@ -3453,53 +3799,59 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>177</v>
-      </c>
-      <c r="B51" t="s">
-        <v>113</v>
+        <v>207</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>149</v>
       </c>
       <c r="C51" t="s">
-        <v>94</v>
+        <v>118</v>
+      </c>
+      <c r="D51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" t="s">
+        <v>224</v>
       </c>
       <c r="G51" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="H51" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>209</v>
-      </c>
-      <c r="B52" t="s">
-        <v>108</v>
+        <v>177</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="G52" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="H52" t="s">
-        <v>204</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>209</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>109</v>
+        <v>177</v>
+      </c>
+      <c r="B53" t="s">
+        <v>113</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="G53" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="H53" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3507,7 +3859,7 @@
         <v>209</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
@@ -3523,8 +3875,8 @@
       <c r="A55" t="s">
         <v>209</v>
       </c>
-      <c r="B55" t="s">
-        <v>111</v>
+      <c r="B55" s="17" t="s">
+        <v>109</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
@@ -3533,70 +3885,61 @@
         <v>89</v>
       </c>
       <c r="H55" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>209</v>
       </c>
-      <c r="B56" s="17" t="s">
-        <v>170</v>
+      <c r="B56" t="s">
+        <v>110</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
       </c>
-      <c r="E56" t="s">
-        <v>231</v>
-      </c>
       <c r="G56" t="s">
         <v>89</v>
       </c>
       <c r="H56" t="s">
-        <v>174</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>208</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>228</v>
+        <v>209</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>118</v>
-      </c>
-      <c r="D57" t="s">
-        <v>41</v>
-      </c>
-      <c r="E57" t="s">
-        <v>227</v>
+        <v>2</v>
       </c>
       <c r="G57" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H57" t="s">
-        <v>87</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="C58" t="s">
-        <v>118</v>
-      </c>
-      <c r="D58" t="s">
-        <v>123</v>
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>231</v>
       </c>
       <c r="G58" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H58" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3604,16 +3947,16 @@
         <v>208</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C59" t="s">
         <v>118</v>
       </c>
       <c r="D59" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="E59" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G59" t="s">
         <v>86</v>
@@ -3627,28 +3970,71 @@
         <v>208</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
       <c r="C60" t="s">
         <v>118</v>
       </c>
       <c r="D60" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" t="s">
-        <v>226</v>
+        <v>123</v>
       </c>
       <c r="G60" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="H60" t="s">
         <v>197</v>
       </c>
     </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>208</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C61" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" t="s">
+        <v>123</v>
+      </c>
+      <c r="E61" t="s">
+        <v>230</v>
+      </c>
+      <c r="G61" t="s">
+        <v>86</v>
+      </c>
+      <c r="H61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>208</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C62" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" t="s">
+        <v>226</v>
+      </c>
+      <c r="G62" t="s">
+        <v>77</v>
+      </c>
+      <c r="H62" t="s">
+        <v>197</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:H60">
+  <autoFilter ref="A2:H62">
     <filterColumn colId="7">
-      <filters>
+      <filters blank="1">
         <filter val="1st ballot"/>
         <filter val="Draft"/>
         <filter val="Proposed"/>
@@ -3663,12 +4049,30 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:C60">
+  <conditionalFormatting sqref="I5:W62">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+      <formula>AND($J$1&gt;=I$4,OR(I5="",I5="Started",I5="Draft"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+      <formula>AND($J$1&gt;=I$3,OR(I5="",I5="Started"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>AND($I$1&gt;=I$4,OR(I5="",I5="Started",I5="Draft"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>AND($I$1&gt;=I$3,OR(I5="",I5="Started"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C5:C62">
       <formula1>WorkGroups</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:W62">
+      <formula1>"Started,Draft,Complete,Reviewed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated Resource names for OO resources
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1061 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/governance/FMG/FMG Tracking Sheet.xlsx
+++ b/documents/governance/FMG/FMG Tracking Sheet.xlsx
@@ -320,9 +320,6 @@
     <t>Connectathon</t>
   </si>
   <si>
-    <t>LabReport</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
@@ -831,6 +828,9 @@
   </si>
   <si>
     <t>Mappings</t>
+  </si>
+  <si>
+    <t>DiagnosticReport</t>
   </si>
 </sst>
 </file>
@@ -1042,9 +1042,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1054,11 +1051,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1084,111 +1084,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1515,7 +1410,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>46</v>
@@ -1527,16 +1422,16 @@
         <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>43</v>
@@ -1544,10 +1439,10 @@
     </row>
     <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>49</v>
@@ -1581,16 +1476,16 @@
         <v>9</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>48</v>
@@ -1601,7 +1496,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>11</v>
@@ -1620,15 +1515,15 @@
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>12</v>
@@ -1652,16 +1547,16 @@
     </row>
     <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>49</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>6</v>
@@ -1674,7 +1569,7 @@
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1691,7 +1586,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>71</v>
@@ -1709,16 +1604,16 @@
         <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>71</v>
@@ -1728,15 +1623,15 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>10</v>
@@ -1763,7 +1658,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>49</v>
@@ -1778,10 +1673,10 @@
         <v>44</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>51</v>
@@ -1807,10 +1702,10 @@
         <v>44</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>68</v>
@@ -1821,7 +1716,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>11</v>
@@ -1840,7 +1735,7 @@
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1854,7 +1749,7 @@
         <v>49</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>8</v>
@@ -1866,7 +1761,7 @@
         <v>49</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>78</v>
@@ -1883,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>71</v>
@@ -1896,15 +1791,15 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>12</v>
@@ -1928,10 +1823,10 @@
     </row>
     <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>12</v>
@@ -1955,10 +1850,10 @@
     </row>
     <row r="17" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>10</v>
@@ -1977,15 +1872,15 @@
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>12</v>
@@ -2000,7 +1895,7 @@
         <v>44</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>7</v>
@@ -2020,7 +1915,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>9</v>
@@ -2029,10 +1924,10 @@
         <v>44</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>67</v>
@@ -2043,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>10</v>
@@ -2058,10 +1953,10 @@
         <v>44</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>67</v>
@@ -2072,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>11</v>
@@ -2116,7 +2011,7 @@
         <v>44</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>6</v>
@@ -2127,10 +2022,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>11</v>
@@ -2139,19 +2034,19 @@
         <v>40</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I23" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -2168,7 +2063,7 @@
         <v>9</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>71</v>
@@ -2183,10 +2078,10 @@
     </row>
     <row r="25" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>11</v>
@@ -2198,7 +2093,7 @@
         <v>40</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -2208,10 +2103,10 @@
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>12</v>
@@ -2244,7 +2139,7 @@
         <v>12</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>9</v>
@@ -2262,10 +2157,10 @@
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>12</v>
@@ -2328,7 +2223,7 @@
         <v>9</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>71</v>
@@ -2352,7 +2247,7 @@
         <v>37</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E31" s="23" t="s">
         <v>7</v>
@@ -2373,7 +2268,7 @@
         <v>24</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>12</v>
@@ -2492,7 +2387,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>11</v>
@@ -2511,7 +2406,7 @@
         <v>20</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>11</v>
@@ -2530,7 +2425,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>11</v>
@@ -2549,7 +2444,7 @@
         <v>25</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>10</v>
@@ -2565,10 +2460,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>10</v>
@@ -2699,10 +2594,10 @@
   <dimension ref="A1:W62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomRight" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2722,47 +2617,47 @@
     <col min="20" max="20" width="10.7109375" customWidth="1"/>
     <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.5703125" customWidth="1"/>
-    <col min="24" max="16384" width="8.85546875" style="26"/>
+    <col min="24" max="16384" width="8.85546875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="30">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="29">
         <f ca="1">TODAY()</f>
-        <v>41330</v>
-      </c>
-      <c r="J1" s="30">
+        <v>41351</v>
+      </c>
+      <c r="J1" s="29">
         <f ca="1">DATE(YEAR($I$1),MONTH($I$1)-1,DAY($I$1))</f>
-        <v>41299</v>
+        <v>41323</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>180</v>
-      </c>
       <c r="E2" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>83</v>
@@ -2771,181 +2666,181 @@
         <v>84</v>
       </c>
       <c r="I2" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="N2" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="O2" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="P2" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="Q2" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="R2" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="S2" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="S2" s="18" t="s">
+      <c r="T2" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="T2" s="18" t="s">
+      <c r="U2" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="U2" s="18" t="s">
+      <c r="V2" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="V2" s="18" t="s">
+      <c r="W2" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="W2" s="18" t="s">
-        <v>267</v>
-      </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29">
+      <c r="B3" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28">
         <v>41334</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="28">
         <v>41334</v>
       </c>
-      <c r="K3" s="29">
+      <c r="K3" s="28">
         <v>41334</v>
       </c>
-      <c r="L3" s="29">
+      <c r="L3" s="28">
         <v>41334</v>
       </c>
-      <c r="M3" s="29">
+      <c r="M3" s="28">
         <v>41365</v>
       </c>
-      <c r="N3" s="29">
+      <c r="N3" s="28">
         <v>41365</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="28">
         <v>41365</v>
       </c>
-      <c r="P3" s="29">
+      <c r="P3" s="28">
         <v>41395</v>
       </c>
-      <c r="Q3" s="29">
+      <c r="Q3" s="28">
         <v>41395</v>
       </c>
-      <c r="R3" s="29">
+      <c r="R3" s="28">
         <v>41395</v>
       </c>
-      <c r="S3" s="29">
+      <c r="S3" s="28">
         <v>41395</v>
       </c>
-      <c r="T3" s="29">
+      <c r="T3" s="28">
         <v>41395</v>
       </c>
-      <c r="U3" s="29">
+      <c r="U3" s="28">
         <v>41395</v>
       </c>
-      <c r="V3" s="29">
+      <c r="V3" s="28">
         <v>41395</v>
       </c>
-      <c r="W3" s="29">
+      <c r="W3" s="28">
         <v>41395</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29">
+      <c r="B4" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28">
         <v>41365</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="28">
         <v>41365</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="28">
         <v>41365</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="28">
         <v>41365</v>
       </c>
-      <c r="M4" s="29">
+      <c r="M4" s="28">
         <v>41395</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="28">
         <v>41395</v>
       </c>
-      <c r="O4" s="29">
+      <c r="O4" s="28">
         <v>41395</v>
       </c>
-      <c r="P4" s="29">
+      <c r="P4" s="28">
         <v>41456</v>
       </c>
-      <c r="Q4" s="29">
+      <c r="Q4" s="28">
         <v>41456</v>
       </c>
-      <c r="R4" s="29">
+      <c r="R4" s="28">
         <v>41456</v>
       </c>
-      <c r="S4" s="29">
+      <c r="S4" s="28">
         <v>41456</v>
       </c>
-      <c r="T4" s="29">
+      <c r="T4" s="28">
         <v>41456</v>
       </c>
-      <c r="U4" s="29">
+      <c r="U4" s="28">
         <v>41456</v>
       </c>
-      <c r="V4" s="29">
+      <c r="V4" s="28">
         <v>41456</v>
       </c>
-      <c r="W4" s="29">
+      <c r="W4" s="28">
         <v>41456</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H5" t="s">
         <v>87</v>
@@ -2953,33 +2848,33 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" t="s">
         <v>188</v>
       </c>
-      <c r="B7" t="s">
-        <v>189</v>
-      </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H7" t="s">
         <v>87</v>
@@ -2987,16 +2882,16 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H8" t="s">
         <v>87</v>
@@ -3004,16 +2899,16 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H9" t="s">
         <v>87</v>
@@ -3021,33 +2916,33 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H11" t="s">
         <v>87</v>
@@ -3055,16 +2950,16 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H12" t="s">
         <v>87</v>
@@ -3072,13 +2967,13 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H13" t="s">
         <v>87</v>
@@ -3086,16 +2981,16 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H14" t="s">
         <v>87</v>
@@ -3103,13 +2998,13 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" t="s">
         <v>183</v>
       </c>
-      <c r="B15" t="s">
-        <v>184</v>
-      </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H15" t="s">
         <v>87</v>
@@ -3117,16 +3012,16 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H16" t="s">
         <v>87</v>
@@ -3134,47 +3029,47 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" t="s">
+        <v>218</v>
+      </c>
+      <c r="G17" t="s">
         <v>98</v>
       </c>
-      <c r="E17" t="s">
-        <v>219</v>
-      </c>
-      <c r="G17" t="s">
-        <v>99</v>
-      </c>
       <c r="H17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G18" t="s">
         <v>38</v>
       </c>
       <c r="H18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>95</v>
@@ -3186,241 +3081,241 @@
         <v>96</v>
       </c>
       <c r="H19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" t="s">
         <v>103</v>
-      </c>
-      <c r="C20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" t="s">
-        <v>104</v>
       </c>
       <c r="G20" t="s">
         <v>89</v>
       </c>
       <c r="H20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G22" t="s">
         <v>89</v>
       </c>
       <c r="H22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" t="s">
         <v>98</v>
       </c>
-      <c r="G23" t="s">
-        <v>99</v>
-      </c>
       <c r="H23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" t="s">
         <v>98</v>
       </c>
-      <c r="G24" t="s">
-        <v>99</v>
-      </c>
       <c r="H24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s">
+        <v>217</v>
+      </c>
+      <c r="G25" t="s">
         <v>98</v>
       </c>
-      <c r="E25" t="s">
-        <v>218</v>
-      </c>
-      <c r="G25" t="s">
-        <v>99</v>
-      </c>
       <c r="H25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
         <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G26" t="s">
         <v>89</v>
       </c>
       <c r="H26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
         <v>94</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G27" t="s">
         <v>89</v>
       </c>
       <c r="H27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G28" t="s">
         <v>89</v>
       </c>
       <c r="H28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G29" t="s">
         <v>89</v>
       </c>
       <c r="H29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G30" t="s">
         <v>38</v>
       </c>
       <c r="H30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
@@ -3429,66 +3324,66 @@
         <v>89</v>
       </c>
       <c r="H31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32" t="s">
         <v>239</v>
       </c>
-      <c r="C32" t="s">
-        <v>119</v>
-      </c>
-      <c r="G32" t="s">
-        <v>240</v>
-      </c>
       <c r="H32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
@@ -3497,75 +3392,75 @@
         <v>89</v>
       </c>
       <c r="H35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C36" t="s">
         <v>93</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G36" t="s">
         <v>89</v>
       </c>
       <c r="H36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G37" t="s">
         <v>89</v>
       </c>
       <c r="H37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" t="s">
+        <v>171</v>
+      </c>
+      <c r="G38" t="s">
         <v>115</v>
       </c>
-      <c r="C38" t="s">
-        <v>118</v>
-      </c>
-      <c r="D38" t="s">
-        <v>104</v>
-      </c>
-      <c r="E38" t="s">
-        <v>172</v>
-      </c>
-      <c r="G38" t="s">
-        <v>116</v>
-      </c>
       <c r="H38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
         <v>94</v>
@@ -3574,41 +3469,41 @@
         <v>89</v>
       </c>
       <c r="H39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G40" t="s">
         <v>89</v>
       </c>
       <c r="H40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E41" t="s">
         <v>7</v>
@@ -3617,15 +3512,15 @@
         <v>89</v>
       </c>
       <c r="H41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
         <v>92</v>
@@ -3634,21 +3529,21 @@
         <v>89</v>
       </c>
       <c r="H42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G43" t="s">
         <v>86</v>
@@ -3659,33 +3554,33 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G44" t="s">
         <v>89</v>
       </c>
       <c r="H44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s">
         <v>94</v>
@@ -3694,18 +3589,18 @@
         <v>86</v>
       </c>
       <c r="H45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D46" t="s">
         <v>94</v>
@@ -3714,21 +3609,21 @@
         <v>86</v>
       </c>
       <c r="H46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>88</v>
       </c>
       <c r="C47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G47" t="s">
         <v>86</v>
@@ -3739,56 +3634,56 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G48" t="s">
         <v>86</v>
       </c>
       <c r="H48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G49" t="s">
         <v>77</v>
       </c>
       <c r="H49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>90</v>
       </c>
       <c r="C50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G50" t="s">
         <v>86</v>
@@ -3799,33 +3694,33 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D51" t="s">
         <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G51" t="s">
         <v>77</v>
       </c>
       <c r="H51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>97</v>
+        <v>267</v>
       </c>
       <c r="C52" t="s">
         <v>94</v>
@@ -3839,27 +3734,27 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C53" t="s">
         <v>94</v>
       </c>
       <c r="G53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
@@ -3868,15 +3763,15 @@
         <v>89</v>
       </c>
       <c r="H54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
@@ -3885,15 +3780,15 @@
         <v>89</v>
       </c>
       <c r="H55" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
@@ -3902,15 +3797,15 @@
         <v>89</v>
       </c>
       <c r="H56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
@@ -3919,44 +3814,44 @@
         <v>89</v>
       </c>
       <c r="H57" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G58" t="s">
         <v>89</v>
       </c>
       <c r="H58" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D59" t="s">
         <v>41</v>
       </c>
       <c r="E59" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G59" t="s">
         <v>86</v>
@@ -3967,39 +3862,39 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G60" t="s">
         <v>86</v>
       </c>
       <c r="H60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B61" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C61" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" t="s">
+        <v>122</v>
+      </c>
+      <c r="E61" t="s">
         <v>229</v>
-      </c>
-      <c r="C61" t="s">
-        <v>118</v>
-      </c>
-      <c r="D61" t="s">
-        <v>123</v>
-      </c>
-      <c r="E61" t="s">
-        <v>230</v>
       </c>
       <c r="G61" t="s">
         <v>86</v>
@@ -4010,25 +3905,25 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D62" t="s">
         <v>77</v>
       </c>
       <c r="E62" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G62" t="s">
         <v>77</v>
       </c>
       <c r="H62" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4118,12 +4013,12 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -4133,12 +4028,12 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>